<commit_message>
Fix bucket search and add cache revalidation for Ultimate UNIQORNs
Bucket search fix:
- Update README to use Python script (generate_frontend_bucket_db.py) instead of node script
- Python script reads from master_bucket_database.json with ALL season games (20,423 games)
- Node script was only reading UNIQORN games (250 games), causing empty bucket results
- Increase bucket-search rate limit from 60 to 200 requests/min for slider interactions

Cache revalidation:
- Add 5-minute revalidation to home page, ultimate page, and player profiles
- Ensures new Ultimate UNIQORN games appear immediately after daily pipeline runs
- Fixes issue where Jokic's new Ultimate UNIQORN showed on home but not ultimate page

Daily workflow:
- Step 3 now runs: python generate_frontend_bucket_db.py
- Removed outdated node script reference
- Updated one-liner command for daily updates
</commit_message>
<xml_diff>
--- a/Ultimate_Uniqorn_Leaderboard_Master.xlsx
+++ b/Ultimate_Uniqorn_Leaderboard_Master.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1758,12 +1758,12 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Damian</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Lillard</t>
         </is>
       </c>
       <c r="C89" t="n">
@@ -1773,12 +1773,12 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Damian</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Lillard</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="C90" t="n">
@@ -1938,12 +1938,12 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Quinn</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Pressey</t>
+          <t>Buckner</t>
         </is>
       </c>
       <c r="C101" t="n">
@@ -1953,12 +1953,12 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Quinn</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>Buckner</t>
+          <t>Pressey</t>
         </is>
       </c>
       <c r="C102" t="n">
@@ -2028,12 +2028,12 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Brook</t>
+          <t>Nikola</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Lopez</t>
+          <t>Jokić</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -2103,12 +2103,12 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Nicolas</t>
+          <t>Brook</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Batum</t>
+          <t>Lopez</t>
         </is>
       </c>
       <c r="C112" t="n">
@@ -2118,12 +2118,12 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Nick</t>
+          <t>Nicolas</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Anderson</t>
+          <t>Batum</t>
         </is>
       </c>
       <c r="C113" t="n">
@@ -2133,12 +2133,12 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Cade</t>
+          <t>Nick</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>Cunningham</t>
+          <t>Anderson</t>
         </is>
       </c>
       <c r="C114" t="n">
@@ -2148,12 +2148,12 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Charles</t>
+          <t>Cade</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Oakley</t>
+          <t>Cunningham</t>
         </is>
       </c>
       <c r="C115" t="n">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Oakley</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -2178,12 +2178,12 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Moussa</t>
+          <t>Charles</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Diabate</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C117" t="n">
@@ -2193,12 +2193,12 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Charlie</t>
+          <t>Moussa</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>Ward</t>
+          <t>Diabate</t>
         </is>
       </c>
       <c r="C118" t="n">
@@ -2208,12 +2208,12 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Chris</t>
+          <t>Charlie</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Mullin</t>
+          <t>Ward</t>
         </is>
       </c>
       <c r="C119" t="n">
@@ -2223,12 +2223,12 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Monta</t>
+          <t>Chris</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>Ellis</t>
+          <t>Mullin</t>
         </is>
       </c>
       <c r="C120" t="n">
@@ -2238,12 +2238,12 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Monta</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Woodson</t>
+          <t>Ellis</t>
         </is>
       </c>
       <c r="C121" t="n">
@@ -2258,7 +2258,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>Gale</t>
+          <t>Woodson</t>
         </is>
       </c>
       <c r="C122" t="n">
@@ -2708,7 +2708,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Robinson</t>
+          <t>Ray</t>
         </is>
       </c>
       <c r="C152" t="n">
@@ -2748,12 +2748,12 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Clifford</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Ray</t>
+          <t>Gale</t>
         </is>
       </c>
       <c r="C155" t="n">
@@ -2778,12 +2778,12 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Michael</t>
+          <t>Clifford</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Cooper</t>
+          <t>Robinson</t>
         </is>
       </c>
       <c r="C157" t="n">
@@ -2793,12 +2793,12 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Eddie</t>
+          <t>Michael</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Jones</t>
+          <t>Cooper</t>
         </is>
       </c>
       <c r="C158" t="n">
@@ -2813,7 +2813,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Wall</t>
         </is>
       </c>
       <c r="C159" t="n">
@@ -2828,7 +2828,7 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Drew</t>
+          <t>Lucas</t>
         </is>
       </c>
       <c r="C160" t="n">
@@ -2838,12 +2838,12 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>English</t>
+          <t>Drew</t>
         </is>
       </c>
       <c r="C161" t="n">
@@ -2853,12 +2853,12 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>Joe</t>
+          <t>Alex</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>English</t>
         </is>
       </c>
       <c r="C162" t="n">
@@ -2868,12 +2868,12 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>Joakim</t>
+          <t>Joe</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="C163" t="n">
@@ -2883,12 +2883,12 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Jimmy</t>
+          <t>Joakim</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Butler</t>
+          <t>Noah</t>
         </is>
       </c>
       <c r="C164" t="n">
@@ -2898,12 +2898,12 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Jim</t>
+          <t>Jimmy</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>Price</t>
+          <t>Butler</t>
         </is>
       </c>
       <c r="C165" t="n">
@@ -2918,7 +2918,7 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>McElroy</t>
+          <t>Price</t>
         </is>
       </c>
       <c r="C166" t="n">
@@ -2928,12 +2928,12 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>Jerry</t>
+          <t>Jim</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>Stackhouse</t>
+          <t>McElroy</t>
         </is>
       </c>
       <c r="C167" t="n">
@@ -2943,12 +2943,12 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>Jerome</t>
+          <t>Jerry</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Stackhouse</t>
         </is>
       </c>
       <c r="C168" t="n">
@@ -2958,12 +2958,12 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>Jeff</t>
+          <t>Jerome</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>Green</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="C169" t="n">
@@ -2973,12 +2973,12 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>Earl</t>
+          <t>Jeff</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Tatum</t>
+          <t>Green</t>
         </is>
       </c>
       <c r="C170" t="n">
@@ -2988,12 +2988,12 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>James</t>
+          <t>Earl</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Tatum</t>
         </is>
       </c>
       <c r="C171" t="n">
@@ -3003,12 +3003,12 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>Jamal</t>
+          <t>James</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Murray</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="C172" t="n">
@@ -3018,12 +3018,12 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Eddie</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Wetzel</t>
+          <t>Jones</t>
         </is>
       </c>
       <c r="C173" t="n">
@@ -3033,12 +3033,12 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>Jamaal</t>
+          <t>Jamal</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Tinsley</t>
+          <t>Murray</t>
         </is>
       </c>
       <c r="C174" t="n">
@@ -3048,12 +3048,12 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>Jalen</t>
+          <t>Jamaal</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Rose</t>
+          <t>Tinsley</t>
         </is>
       </c>
       <c r="C175" t="n">
@@ -3068,7 +3068,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Rose</t>
         </is>
       </c>
       <c r="C176" t="n">
@@ -3078,12 +3078,12 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>Hot</t>
+          <t>Jalen</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Rod Williams</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="C177" t="n">
@@ -3093,12 +3093,12 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>Hersey</t>
+          <t>Hot</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Hawkins</t>
+          <t>Rod Williams</t>
         </is>
       </c>
       <c r="C178" t="n">
@@ -3108,12 +3108,12 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>Elfrid</t>
+          <t>Hersey</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Payton</t>
+          <t>Hawkins</t>
         </is>
       </c>
       <c r="C179" t="n">
@@ -3123,12 +3123,12 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>Greg</t>
+          <t>Elfrid</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Stiemsma</t>
+          <t>Payton</t>
         </is>
       </c>
       <c r="C180" t="n">
@@ -3143,7 +3143,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Ostertag</t>
+          <t>Stiemsma</t>
         </is>
       </c>
       <c r="C181" t="n">
@@ -3153,12 +3153,12 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>Elliot</t>
+          <t>Greg</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Perry</t>
+          <t>Ostertag</t>
         </is>
       </c>
       <c r="C182" t="n">
@@ -3168,12 +3168,12 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>Elton</t>
+          <t>Elliot</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Brand</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C183" t="n">
@@ -3183,12 +3183,12 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>George</t>
+          <t>Elton</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Gervin</t>
+          <t>Brand</t>
         </is>
       </c>
       <c r="C184" t="n">
@@ -3198,12 +3198,12 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Garfield</t>
+          <t>George</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Heard</t>
+          <t>Gervin</t>
         </is>
       </c>
       <c r="C185" t="n">
@@ -3213,12 +3213,12 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>Fred</t>
+          <t>Garfield</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>VanVleet</t>
+          <t>Heard</t>
         </is>
       </c>
       <c r="C186" t="n">
@@ -3228,12 +3228,12 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Fred</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Wall</t>
+          <t>VanVleet</t>
         </is>
       </c>
       <c r="C187" t="n">
@@ -3243,12 +3243,12 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>Jrue</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Wetzel</t>
         </is>
       </c>
       <c r="C188" t="n">
@@ -3258,12 +3258,12 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>Metta</t>
+          <t>Jrue</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>World Peace</t>
+          <t>Holiday</t>
         </is>
       </c>
       <c r="C189" t="n">
@@ -3273,12 +3273,12 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>Larry</t>
+          <t>Juan</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Kenon</t>
+          <t>Dixon</t>
         </is>
       </c>
       <c r="C190" t="n">
@@ -3288,12 +3288,12 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>Corey</t>
+          <t>Darnell</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Brewer</t>
+          <t>Hillman</t>
         </is>
       </c>
       <c r="C191" t="n">
@@ -3303,12 +3303,12 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>Mark</t>
+          <t>Metta</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Davis</t>
+          <t>World Peace</t>
         </is>
       </c>
       <c r="C192" t="n">
@@ -3318,12 +3318,12 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>Mario</t>
+          <t>Corey</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Chalmers</t>
+          <t>Brewer</t>
         </is>
       </c>
       <c r="C193" t="n">
@@ -3333,12 +3333,12 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>Eric</t>
+          <t>Mark</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Snow</t>
+          <t>Davis</t>
         </is>
       </c>
       <c r="C194" t="n">
@@ -3348,12 +3348,12 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>Marc</t>
+          <t>Mario</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Gasol</t>
+          <t>Chalmers</t>
         </is>
       </c>
       <c r="C195" t="n">
@@ -3363,12 +3363,12 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>Manute</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Bol</t>
+          <t>Snow</t>
         </is>
       </c>
       <c r="C196" t="n">
@@ -3378,12 +3378,12 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>Curtis</t>
+          <t>Marc</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Perry</t>
+          <t>Gasol</t>
         </is>
       </c>
       <c r="C197" t="n">
@@ -3393,12 +3393,12 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>Lou</t>
+          <t>Manute</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>Williams</t>
+          <t>Bol</t>
         </is>
       </c>
       <c r="C198" t="n">
@@ -3408,12 +3408,12 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>Dan</t>
+          <t>Curtis</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>Issel</t>
+          <t>Perry</t>
         </is>
       </c>
       <c r="C199" t="n">
@@ -3423,12 +3423,12 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>Lionel</t>
+          <t>Lou</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Simmons</t>
+          <t>Williams</t>
         </is>
       </c>
       <c r="C200" t="n">
@@ -3438,12 +3438,12 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>Lionel</t>
+          <t>Dan</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Hollins</t>
+          <t>Issel</t>
         </is>
       </c>
       <c r="C201" t="n">
@@ -3453,12 +3453,12 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>Larry</t>
+          <t>Lionel</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Smith</t>
+          <t>Simmons</t>
         </is>
       </c>
       <c r="C202" t="n">
@@ -3468,12 +3468,12 @@
     <row r="203">
       <c r="A203" t="inlineStr">
         <is>
-          <t>Darnell</t>
+          <t>Lionel</t>
         </is>
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Hillman</t>
+          <t>Hollins</t>
         </is>
       </c>
       <c r="C203" t="n">
@@ -3483,12 +3483,12 @@
     <row r="204">
       <c r="A204" t="inlineStr">
         <is>
-          <t>Darnell</t>
+          <t>Larry</t>
         </is>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Valentine</t>
+          <t>Smith</t>
         </is>
       </c>
       <c r="C204" t="n">
@@ -3498,12 +3498,12 @@
     <row r="205">
       <c r="A205" t="inlineStr">
         <is>
-          <t>Juan</t>
+          <t>Larry</t>
         </is>
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Dixon</t>
+          <t>Kenon</t>
         </is>
       </c>
       <c r="C205" t="n">
@@ -3513,12 +3513,12 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
-          <t>Lamar</t>
+          <t>Devin</t>
         </is>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Odom</t>
+          <t>Booker</t>
         </is>
       </c>
       <c r="C206" t="n">
@@ -3528,12 +3528,12 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
-          <t>LaMarcus</t>
+          <t>Darnell</t>
         </is>
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Aldridge</t>
+          <t>Valentine</t>
         </is>
       </c>
       <c r="C207" t="n">
@@ -3543,12 +3543,12 @@
     <row r="208">
       <c r="A208" t="inlineStr">
         <is>
-          <t>Kyrie</t>
+          <t>Lamar</t>
         </is>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Irving</t>
+          <t>Odom</t>
         </is>
       </c>
       <c r="C208" t="n">
@@ -3558,12 +3558,12 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Kobe</t>
+          <t>LaMarcus</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Bryant</t>
+          <t>Aldridge</t>
         </is>
       </c>
       <c r="C209" t="n">
@@ -3573,12 +3573,12 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Klay</t>
+          <t>Kyrie</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Thompson</t>
+          <t>Irving</t>
         </is>
       </c>
       <c r="C210" t="n">
@@ -3588,12 +3588,12 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Dave</t>
+          <t>Kobe</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Cowens</t>
+          <t>Bryant</t>
         </is>
       </c>
       <c r="C211" t="n">
@@ -3603,12 +3603,12 @@
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Kevin</t>
+          <t>Klay</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Johnson</t>
+          <t>Thompson</t>
         </is>
       </c>
       <c r="C212" t="n">
@@ -3618,12 +3618,12 @@
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Kendall</t>
+          <t>Dave</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Gill</t>
+          <t>Cowens</t>
         </is>
       </c>
       <c r="C213" t="n">
@@ -3633,12 +3633,12 @@
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Kawhi</t>
+          <t>Kevin</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Leonard</t>
+          <t>Johnson</t>
         </is>
       </c>
       <c r="C214" t="n">
@@ -3648,12 +3648,12 @@
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Karl-Anthony</t>
+          <t>Kendall</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Towns</t>
+          <t>Gill</t>
         </is>
       </c>
       <c r="C215" t="n">
@@ -3663,12 +3663,12 @@
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Derrick</t>
+          <t>Kawhi</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Favors</t>
+          <t>Leonard</t>
         </is>
       </c>
       <c r="C216" t="n">
@@ -3678,12 +3678,12 @@
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Derrick</t>
+          <t>Karl-Anthony</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>White</t>
+          <t>Towns</t>
         </is>
       </c>
       <c r="C217" t="n">
@@ -3693,12 +3693,12 @@
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Devin</t>
+          <t>Derrick</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Booker</t>
+          <t>Favors</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -3708,15 +3708,30 @@
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
+          <t>Derrick</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
+      </c>
+      <c r="C219" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
           <t>Adonal</t>
         </is>
       </c>
-      <c r="B219" t="inlineStr">
+      <c r="B220" t="inlineStr">
         <is>
           <t>Foyle</t>
         </is>
       </c>
-      <c r="C219" t="n">
+      <c r="C220" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>